<commit_message>
Runtime optimizacija pakeista į O3 ir atlikti smulkūs programos papildymai
</commit_message>
<xml_diff>
--- a/spartos-analize/programos-spartos-analize.xlsx
+++ b/spartos-analize/programos-spartos-analize.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mykolasmotiejunas/Documents/vs-git-repositories/objektinis-pirma/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mykolasmotiejunas/Documents/vs-git-repositories/objektinis-pirma/spartos-analize/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{748A8FCC-74BF-764F-9C81-ECA1EDEB9CD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{837F74DB-E56E-3646-B3D3-6DD0266FB970}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16220" xr2:uid="{AEA47B78-08EF-3743-9352-70FFE0876222}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16220" xr2:uid="{AEA47B78-08EF-3743-9352-70FFE0876222}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -468,8 +468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BB18AB8-3974-C64F-83B9-2240ECB77FEA}">
   <dimension ref="D6:N58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="M61" sqref="M61"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49:M49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -866,34 +866,34 @@
     </row>
     <row r="27" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D27">
-        <v>6.1942500000000001E-3</v>
+        <v>9.6252500000000001E-3</v>
       </c>
       <c r="E27">
-        <v>4.4885000000000003E-3</v>
+        <v>6.5814999999999997E-3</v>
       </c>
       <c r="F27">
-        <v>3.01014E-2</v>
+        <v>5.2938199999999998E-2</v>
       </c>
       <c r="G27">
-        <v>2.31922E-2</v>
+        <v>2.93637E-2</v>
       </c>
       <c r="H27">
-        <v>0.26572000000000001</v>
+        <v>0.258162</v>
       </c>
       <c r="I27">
-        <v>0.239977</v>
+        <v>0.21557499999999999</v>
       </c>
       <c r="J27">
-        <v>2.2955000000000001</v>
+        <v>2.1775199999999999</v>
       </c>
       <c r="K27">
-        <v>2.2295799999999999</v>
+        <v>2.1295500000000001</v>
       </c>
       <c r="L27">
-        <v>25.444800000000001</v>
+        <v>23.725100000000001</v>
       </c>
       <c r="M27">
-        <v>23.340499999999999</v>
+        <v>26.2197</v>
       </c>
       <c r="N27" t="s">
         <v>2</v>
@@ -901,34 +901,34 @@
     </row>
     <row r="28" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D28">
-        <v>1.20209E-4</v>
+        <v>4.1733299999999998E-4</v>
       </c>
       <c r="E28">
-        <v>1.10917E-4</v>
+        <v>2.0066600000000001E-4</v>
       </c>
       <c r="F28">
-        <v>6.6387499999999997E-4</v>
+        <v>1.2636699999999999E-3</v>
       </c>
       <c r="G28">
-        <v>1.6973299999999999E-3</v>
+        <v>1.13342E-3</v>
       </c>
       <c r="H28">
-        <v>6.8089200000000004E-3</v>
+        <v>7.1027499999999997E-3</v>
       </c>
       <c r="I28">
-        <v>3.6743499999999998E-2</v>
+        <v>2.09792E-2</v>
       </c>
       <c r="J28">
-        <v>0.101106</v>
+        <v>9.9339899999999995E-2</v>
       </c>
       <c r="K28">
-        <v>0.84311800000000003</v>
+        <v>0.65255799999999997</v>
       </c>
       <c r="L28">
-        <v>0.90696299999999996</v>
+        <v>0.905532</v>
       </c>
       <c r="M28">
-        <v>22.118600000000001</v>
+        <v>12.5252</v>
       </c>
       <c r="N28" t="s">
         <v>3</v>
@@ -936,34 +936,34 @@
     </row>
     <row r="29" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D29">
-        <v>2.8983399999999999E-4</v>
+        <v>2.7845799999999998E-4</v>
       </c>
       <c r="E29">
-        <v>3.19792E-4</v>
+        <v>3.5633399999999998E-4</v>
       </c>
       <c r="F29">
-        <v>1.6764200000000001E-3</v>
+        <v>1.5719600000000001E-3</v>
       </c>
       <c r="G29">
-        <v>2.0855399999999999E-3</v>
+        <v>1.63142E-3</v>
       </c>
       <c r="H29">
-        <v>2.9169E-2</v>
+        <v>1.5906300000000002E-2</v>
       </c>
       <c r="I29">
-        <v>4.8246600000000001E-2</v>
+        <v>2.9835E-2</v>
       </c>
       <c r="J29">
-        <v>0.42185400000000001</v>
+        <v>0.240173</v>
       </c>
       <c r="K29">
-        <v>0.57590300000000005</v>
+        <v>0.55680200000000002</v>
       </c>
       <c r="L29">
-        <v>26.700700000000001</v>
+        <v>5.5067700000000004</v>
       </c>
       <c r="M29">
-        <v>130.083</v>
+        <v>65.600800000000007</v>
       </c>
       <c r="N29" t="s">
         <v>4</v>
@@ -971,34 +971,34 @@
     </row>
     <row r="30" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D30">
-        <v>2.73529E-3</v>
+        <v>1.0889599999999999E-3</v>
       </c>
       <c r="E30">
-        <v>2.4671699999999999E-3</v>
+        <v>7.74458E-4</v>
       </c>
       <c r="F30">
-        <v>1.6187699999999999E-2</v>
+        <v>2.7775399999999998E-3</v>
       </c>
       <c r="G30">
-        <v>1.82089E-2</v>
+        <v>1.8125800000000001E-3</v>
       </c>
       <c r="H30">
-        <v>0.13806499999999999</v>
+        <v>1.5661499999999998E-2</v>
       </c>
       <c r="I30">
-        <v>0.144649</v>
+        <v>2.2657299999999998E-2</v>
       </c>
       <c r="J30">
-        <v>1.5667899999999999</v>
+        <v>0.188666</v>
       </c>
       <c r="K30">
-        <v>1.4005399999999999</v>
+        <v>0.20315900000000001</v>
       </c>
       <c r="L30">
-        <v>15.003399999999999</v>
+        <v>2.0125199999999999</v>
       </c>
       <c r="M30">
-        <v>15.4099</v>
+        <v>2.3549199999999999</v>
       </c>
       <c r="N30" s="1" t="s">
         <v>5</v>
@@ -1006,34 +1006,34 @@
     </row>
     <row r="31" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D31">
-        <v>2.8202100000000001E-3</v>
+        <v>6.8216700000000002E-4</v>
       </c>
       <c r="E31">
-        <v>2.1871199999999999E-3</v>
+        <v>6.1625000000000004E-4</v>
       </c>
       <c r="F31">
-        <v>1.9031900000000001E-2</v>
+        <v>2.1565E-3</v>
       </c>
       <c r="G31">
-        <v>1.50642E-2</v>
+        <v>2.0855800000000001E-3</v>
       </c>
       <c r="H31">
-        <v>0.134238</v>
+        <v>1.51857E-2</v>
       </c>
       <c r="I31">
-        <v>0.144785</v>
+        <v>1.6297699999999998E-2</v>
       </c>
       <c r="J31">
-        <v>1.45133</v>
+        <v>0.13837099999999999</v>
       </c>
       <c r="K31">
-        <v>1.3559000000000001</v>
+        <v>0.195767</v>
       </c>
       <c r="L31">
-        <v>14.518700000000001</v>
+        <v>2.8715600000000001</v>
       </c>
       <c r="M31">
-        <v>15.7272</v>
+        <v>2.3601700000000001</v>
       </c>
       <c r="N31" s="1" t="s">
         <v>6</v>
@@ -1041,34 +1041,34 @@
     </row>
     <row r="32" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D32">
-        <v>1.2203500000000001E-2</v>
+        <v>1.2154999999999999E-2</v>
       </c>
       <c r="E32">
-        <v>9.6102500000000007E-3</v>
+        <v>8.5753700000000006E-3</v>
       </c>
       <c r="F32">
-        <v>6.7709000000000005E-2</v>
+        <v>6.0753399999999999E-2</v>
       </c>
       <c r="G32">
-        <v>6.0303799999999998E-2</v>
+        <v>3.6058600000000003E-2</v>
       </c>
       <c r="H32">
-        <v>0.57408400000000004</v>
+        <v>0.31212499999999999</v>
       </c>
       <c r="I32">
-        <v>0.61448199999999997</v>
+        <v>0.30540899999999999</v>
       </c>
       <c r="J32">
-        <v>5.8366899999999999</v>
+        <v>2.84416</v>
       </c>
       <c r="K32">
-        <v>6.4051400000000003</v>
+        <v>3.7379199999999999</v>
       </c>
       <c r="L32">
-        <v>82.575199999999995</v>
+        <v>35.021599999999999</v>
       </c>
       <c r="M32">
-        <v>206.68</v>
+        <v>109.06100000000001</v>
       </c>
       <c r="N32" t="s">
         <v>9</v>
@@ -1158,34 +1158,34 @@
     </row>
     <row r="40" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D40">
-        <v>9.6822100000000001E-3</v>
+        <v>9.1308299999999995E-3</v>
       </c>
       <c r="E40">
-        <v>6.1026700000000001E-3</v>
+        <v>2.5149199999999999E-3</v>
       </c>
       <c r="F40">
-        <v>5.3296000000000003E-2</v>
+        <v>3.9048199999999998E-2</v>
       </c>
       <c r="G40">
-        <v>2.2137899999999999E-2</v>
+        <v>2.13361E-2</v>
       </c>
       <c r="H40">
-        <v>0.26466600000000001</v>
+        <v>0.25558599999999998</v>
       </c>
       <c r="I40">
-        <v>0.22304299999999999</v>
+        <v>0.29861799999999999</v>
       </c>
       <c r="J40">
         <v>2.2208700000000001</v>
       </c>
       <c r="K40">
-        <v>2.30375</v>
+        <v>2.1996000000000002</v>
       </c>
       <c r="L40">
         <v>24.819800000000001</v>
       </c>
       <c r="M40">
-        <v>23.026900000000001</v>
+        <v>21.8919</v>
       </c>
       <c r="N40" t="s">
         <v>2</v>
@@ -1193,34 +1193,34 @@
     </row>
     <row r="41" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D41">
-        <v>1.96083E-4</v>
+        <v>4.6029099999999999E-4</v>
       </c>
       <c r="E41">
-        <v>1.56334E-4</v>
+        <v>6.084E-5</v>
       </c>
       <c r="F41">
-        <v>1.03921E-3</v>
+        <v>1.3691199999999999E-3</v>
       </c>
       <c r="G41">
-        <v>1.01833E-3</v>
+        <v>8.7495800000000001E-4</v>
       </c>
       <c r="H41">
-        <v>6.2238299999999996E-3</v>
+        <v>8.6944599999999993E-3</v>
       </c>
       <c r="I41">
-        <v>3.2417700000000001E-2</v>
+        <v>2.15617E-2</v>
       </c>
       <c r="J41">
         <v>6.8279999999999993E-2</v>
       </c>
       <c r="K41">
-        <v>0.76752100000000001</v>
+        <v>0.63495800000000002</v>
       </c>
       <c r="L41">
         <v>0.951322</v>
       </c>
       <c r="M41">
-        <v>38.767800000000001</v>
+        <v>14.884600000000001</v>
       </c>
       <c r="N41" t="s">
         <v>3</v>
@@ -1228,34 +1228,34 @@
     </row>
     <row r="42" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D42">
-        <v>1.7502100000000001E-3</v>
+        <v>1.78283E-3</v>
       </c>
       <c r="E42">
-        <v>1.7729200000000001E-4</v>
+        <v>4.2125000000000001E-5</v>
       </c>
       <c r="F42">
-        <v>6.6241700000000001E-2</v>
+        <v>7.4233599999999997E-2</v>
       </c>
       <c r="G42">
-        <v>6.8370799999999999E-4</v>
+        <v>6.6045899999999996E-4</v>
       </c>
       <c r="H42">
-        <v>5.6047700000000003</v>
+        <v>5.7900900000000002</v>
       </c>
       <c r="I42">
-        <v>2.54617E-2</v>
+        <v>1.8127899999999999E-2</v>
       </c>
       <c r="J42" t="s">
         <v>13</v>
       </c>
       <c r="K42">
-        <v>0.28170299999999998</v>
+        <v>0.207813</v>
       </c>
       <c r="L42" t="s">
         <v>13</v>
       </c>
       <c r="M42">
-        <v>32.947699999999998</v>
+        <v>9.4475300000000004</v>
       </c>
       <c r="N42" t="s">
         <v>4</v>
@@ -1263,34 +1263,34 @@
     </row>
     <row r="43" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D43">
-        <v>4.6715799999999998E-3</v>
+        <v>3.7849899999999999E-2</v>
       </c>
       <c r="E43">
-        <v>3.4388299999999999E-3</v>
+        <v>2.4458299999999999E-4</v>
       </c>
       <c r="F43">
-        <v>1.49216E-2</v>
+        <v>2.1755400000000001E-3</v>
       </c>
       <c r="G43">
-        <v>1.3551499999999999E-2</v>
+        <v>1.9497500000000001E-3</v>
       </c>
       <c r="H43">
-        <v>0.141679</v>
+        <v>1.6341499999999998E-2</v>
       </c>
       <c r="I43">
-        <v>0.14622199999999999</v>
+        <v>1.3631000000000001E-2</v>
       </c>
       <c r="J43" t="s">
         <v>13</v>
       </c>
       <c r="K43">
-        <v>1.56711</v>
+        <v>0.15093100000000001</v>
       </c>
       <c r="L43" t="s">
         <v>13</v>
       </c>
       <c r="M43">
-        <v>59.392099999999999</v>
+        <v>9.9357399999999991</v>
       </c>
       <c r="N43" s="1" t="s">
         <v>5</v>
@@ -1298,34 +1298,34 @@
     </row>
     <row r="44" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D44">
-        <v>3.8772899999999998E-3</v>
+        <v>3.2362200000000001E-2</v>
       </c>
       <c r="E44">
-        <v>2.9432500000000001E-3</v>
+        <v>2.5133300000000001E-4</v>
       </c>
       <c r="F44">
-        <v>1.4386599999999999E-2</v>
+        <v>1.60133E-3</v>
       </c>
       <c r="G44">
-        <v>1.3868800000000001E-2</v>
+        <v>3.5526199999999998E-3</v>
       </c>
       <c r="H44">
-        <v>0.13297600000000001</v>
+        <v>1.51515E-2</v>
       </c>
       <c r="I44">
-        <v>0.14013400000000001</v>
+        <v>2.1311799999999999E-2</v>
       </c>
       <c r="J44" t="s">
         <v>13</v>
       </c>
       <c r="K44">
-        <v>1.41126</v>
+        <v>0.23924100000000001</v>
       </c>
       <c r="L44" t="s">
         <v>13</v>
       </c>
       <c r="M44">
-        <v>42.456299999999999</v>
+        <v>14.861499999999999</v>
       </c>
       <c r="N44" s="1" t="s">
         <v>6</v>
@@ -1333,34 +1333,34 @@
     </row>
     <row r="45" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D45">
-        <v>2.0249199999999998E-2</v>
+        <v>8.1677E-2</v>
       </c>
       <c r="E45">
-        <v>1.28577E-2</v>
+        <v>3.1289999999999998E-3</v>
       </c>
       <c r="F45">
-        <v>0.149949</v>
+        <v>0.118482</v>
       </c>
       <c r="G45">
-        <v>5.1294800000000002E-2</v>
+        <v>2.84026E-2</v>
       </c>
       <c r="H45">
-        <v>6.1503899999999998</v>
+        <v>6.0860300000000001</v>
       </c>
       <c r="I45">
-        <v>0.56735199999999997</v>
+        <v>0.37331199999999998</v>
       </c>
       <c r="J45" t="s">
         <v>13</v>
       </c>
       <c r="K45">
-        <v>6.3314599999999999</v>
+        <v>3.4326300000000001</v>
       </c>
       <c r="L45" t="s">
         <v>13</v>
       </c>
       <c r="M45">
-        <v>196.59100000000001</v>
+        <v>70.997600000000006</v>
       </c>
       <c r="N45" t="s">
         <v>9</v>
@@ -1464,34 +1464,34 @@
     </row>
     <row r="53" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D53">
-        <v>9.8051700000000002E-3</v>
+        <v>9.2640399999999994E-3</v>
       </c>
       <c r="E53">
-        <v>6.0431699999999996E-3</v>
+        <v>6.5449999999999996E-3</v>
       </c>
       <c r="F53">
-        <v>5.3897199999999999E-2</v>
+        <v>5.2044800000000002E-2</v>
       </c>
       <c r="G53">
-        <v>2.35877E-2</v>
+        <v>2.7611E-2</v>
       </c>
       <c r="H53">
-        <v>0.26741900000000002</v>
+        <v>0.25426199999999999</v>
       </c>
       <c r="I53">
-        <v>0.33307700000000001</v>
+        <v>0.34542800000000001</v>
       </c>
       <c r="J53">
-        <v>2.2680199999999999</v>
+        <v>2.1598700000000002</v>
       </c>
       <c r="K53">
-        <v>2.2116899999999999</v>
+        <v>2.1947899999999998</v>
       </c>
       <c r="L53">
-        <v>24.868200000000002</v>
+        <v>24.0488</v>
       </c>
       <c r="M53">
-        <v>23.525600000000001</v>
+        <v>22.1267</v>
       </c>
       <c r="N53" t="s">
         <v>2</v>
@@ -1499,34 +1499,34 @@
     </row>
     <row r="54" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D54">
-        <v>1.9316599999999999E-4</v>
+        <v>4.3108399999999998E-4</v>
       </c>
       <c r="E54">
-        <v>1.7145800000000001E-4</v>
+        <v>1.5129100000000001E-4</v>
       </c>
       <c r="F54">
-        <v>1.0235400000000001E-3</v>
+        <v>1.2318299999999999E-3</v>
       </c>
       <c r="G54">
-        <v>1.1745799999999999E-3</v>
+        <v>1.0512900000000001E-3</v>
       </c>
       <c r="H54">
-        <v>7.2672500000000003E-3</v>
+        <v>7.0575000000000004E-3</v>
       </c>
       <c r="I54">
-        <v>3.1710200000000001E-2</v>
+        <v>2.1521499999999999E-2</v>
       </c>
       <c r="J54">
-        <v>0.10247299999999999</v>
+        <v>6.7564700000000005E-2</v>
       </c>
       <c r="K54">
-        <v>0.76694799999999996</v>
+        <v>0.65173899999999996</v>
       </c>
       <c r="L54">
-        <v>0.93411900000000003</v>
+        <v>0.89059500000000003</v>
       </c>
       <c r="M54">
-        <v>16.495000000000001</v>
+        <v>28.8428</v>
       </c>
       <c r="N54" t="s">
         <v>3</v>
@@ -1534,34 +1534,34 @@
     </row>
     <row r="55" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D55">
-        <v>2.0491699999999999E-4</v>
+        <v>1.4637499999999999E-4</v>
       </c>
       <c r="E55">
-        <v>3.7733299999999999E-4</v>
+        <v>1.3479099999999999E-4</v>
       </c>
       <c r="F55">
-        <v>1.14533E-3</v>
+        <v>5.8333300000000001E-4</v>
       </c>
       <c r="G55">
-        <v>8.9375000000000001E-4</v>
+        <v>6.5824999999999998E-4</v>
       </c>
       <c r="H55">
-        <v>1.0344000000000001E-2</v>
+        <v>5.7080799999999999E-3</v>
       </c>
       <c r="I55">
-        <v>2.6686399999999999E-2</v>
+        <v>1.5738700000000001E-2</v>
       </c>
       <c r="J55">
-        <v>0.22517499999999999</v>
+        <v>0.10440199999999999</v>
       </c>
       <c r="K55">
-        <v>0.27585799999999999</v>
+        <v>0.20430300000000001</v>
       </c>
       <c r="L55">
-        <v>5.4665999999999997</v>
+        <v>1.9609300000000001</v>
       </c>
       <c r="M55">
-        <v>3.8739400000000002</v>
+        <v>20.4863</v>
       </c>
       <c r="N55" t="s">
         <v>4</v>
@@ -1569,34 +1569,34 @@
     </row>
     <row r="56" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D56">
-        <v>6.2521199999999999E-3</v>
+        <v>1.7279999999999999E-3</v>
       </c>
       <c r="E56">
-        <v>3.97125E-3</v>
+        <v>5.8012500000000002E-4</v>
       </c>
       <c r="F56">
-        <v>2.4501100000000001E-2</v>
+        <v>2.54967E-3</v>
       </c>
       <c r="G56">
-        <v>1.3133000000000001E-2</v>
+        <v>1.4589200000000001E-3</v>
       </c>
       <c r="H56">
-        <v>0.131468</v>
+        <v>1.6496899999999998E-2</v>
       </c>
       <c r="I56">
-        <v>0.13878099999999999</v>
+        <v>1.54769E-2</v>
       </c>
       <c r="J56">
-        <v>1.3029200000000001</v>
+        <v>0.13977700000000001</v>
       </c>
       <c r="K56">
-        <v>1.7654700000000001</v>
+        <v>0.14511199999999999</v>
       </c>
       <c r="L56">
-        <v>13.4763</v>
+        <v>2.4588000000000001</v>
       </c>
       <c r="M56">
-        <v>27.3931</v>
+        <v>11.2874</v>
       </c>
       <c r="N56" s="1" t="s">
         <v>5</v>
@@ -1604,34 +1604,34 @@
     </row>
     <row r="57" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D57">
-        <v>4.3512100000000003E-3</v>
+        <v>9.3004100000000005E-4</v>
       </c>
       <c r="E57">
-        <v>3.3080399999999999E-3</v>
+        <v>5.2608400000000001E-4</v>
       </c>
       <c r="F57">
-        <v>1.6129000000000001E-2</v>
+        <v>2.15525E-3</v>
       </c>
       <c r="G57">
-        <v>1.33826E-2</v>
+        <v>2.1247100000000001E-3</v>
       </c>
       <c r="H57">
-        <v>0.24635399999999999</v>
+        <v>1.4209599999999999E-2</v>
       </c>
       <c r="I57">
-        <v>0.14485999999999999</v>
+        <v>1.96711E-2</v>
       </c>
       <c r="J57">
-        <v>1.4527000000000001</v>
+        <v>0.16389599999999999</v>
       </c>
       <c r="K57">
-        <v>1.5986400000000001</v>
+        <v>0.249253</v>
       </c>
       <c r="L57">
-        <v>15.844099999999999</v>
+        <v>3.4760399999999998</v>
       </c>
       <c r="M57">
-        <v>27.226199999999999</v>
+        <v>12.391</v>
       </c>
       <c r="N57" s="1" t="s">
         <v>6</v>
@@ -1639,34 +1639,34 @@
     </row>
     <row r="58" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D58">
-        <v>2.08723E-2</v>
+        <v>1.2568299999999999E-2</v>
       </c>
       <c r="E58">
-        <v>1.39217E-2</v>
+        <v>7.9770399999999995E-3</v>
       </c>
       <c r="F58">
-        <v>9.6760700000000005E-2</v>
+        <v>5.8606499999999999E-2</v>
       </c>
       <c r="G58">
-        <v>5.22076E-2</v>
+        <v>3.2927400000000003E-2</v>
       </c>
       <c r="H58">
-        <v>0.66292499999999999</v>
+        <v>0.29780699999999999</v>
       </c>
       <c r="I58">
-        <v>0.67520400000000003</v>
+        <v>0.417904</v>
       </c>
       <c r="J58">
-        <v>5.3513799999999998</v>
+        <v>2.6355900000000001</v>
       </c>
       <c r="K58">
-        <v>6.6186800000000003</v>
+        <v>3.4452600000000002</v>
       </c>
       <c r="L58">
-        <v>60.589799999999997</v>
+        <v>32.835299999999997</v>
       </c>
       <c r="M58">
-        <v>98.513900000000007</v>
+        <v>95.134200000000007</v>
       </c>
       <c r="N58" t="s">
         <v>9</v>
@@ -1674,14 +1674,17 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="D46:M46"/>
-    <mergeCell ref="D49:M49"/>
-    <mergeCell ref="D50:M50"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="H51:I51"/>
-    <mergeCell ref="J51:K51"/>
-    <mergeCell ref="L51:M51"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="D6:M6"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
     <mergeCell ref="D23:M23"/>
     <mergeCell ref="D36:M36"/>
     <mergeCell ref="D38:E38"/>
@@ -1695,18 +1698,15 @@
     <mergeCell ref="H25:I25"/>
     <mergeCell ref="J25:K25"/>
     <mergeCell ref="L25:M25"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="D6:M6"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
     <mergeCell ref="D37:M37"/>
+    <mergeCell ref="D46:M46"/>
+    <mergeCell ref="D49:M49"/>
+    <mergeCell ref="D50:M50"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="H51:I51"/>
+    <mergeCell ref="J51:K51"/>
+    <mergeCell ref="L51:M51"/>
   </mergeCells>
   <conditionalFormatting sqref="D10:D15">
     <cfRule type="colorScale" priority="11">
@@ -1717,6 +1717,18 @@
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D40:K45">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
@@ -1768,18 +1780,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D40:K45">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="D53:M58">
     <cfRule type="colorScale" priority="1">
       <colorScale>

</xml_diff>